<commit_message>
update upload and query
</commit_message>
<xml_diff>
--- a/app/files/wto.xlsx
+++ b/app/files/wto.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="69">
   <si>
     <t>import</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>request_print_date</t>
+  </si>
+  <si>
+    <t>custom_print_date</t>
   </si>
 </sst>
 </file>
@@ -892,199 +895,212 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.125" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.125" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.125" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6">
+        <v>42791</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>46</v>
       </c>
       <c r="E2" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="6">
         <v>42756</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>42</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>28</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>41</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>36.0852</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>36000</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>1299067.2</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>25000</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6">
+        <v>42792</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
       </c>
       <c r="E3" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="6">
         <v>42757</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>60</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>28</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>41</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>36.0852</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>36000</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>1299067.2</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>25000</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6">
+        <v>42793</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
       </c>
       <c r="E4" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="6">
         <v>42758</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>61</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>28</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>41</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>36.0852</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>36000</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>1299067.2</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>25000</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update in & out quota
</commit_message>
<xml_diff>
--- a/app/files/wto.xlsx
+++ b/app/files/wto.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="108">
   <si>
     <t>import</t>
   </si>
@@ -180,24 +180,6 @@
     <t>037496</t>
   </si>
   <si>
-    <t>RICEGROWERS SINGAPORE PTE LIMITED T/AS SUNRICE LEVEL 20-61 ONE RAFFLES PLACE TOWER 2 SINGAPORE SLO48617</t>
-  </si>
-  <si>
-    <t>75/27-29 ชั้นที่ 18-19 อาคารโอเชี่ยนทาวเวอร์ 2 ซอยสุขุมวิท 19 (ซอยวัฒนา) ถนนสุขุมวิท แขวงคลองเตยเหนือ เขตวัฒนา กรุงเทพมหานคร 10111</t>
-  </si>
-  <si>
-    <t>0-2259-7871-9</t>
-  </si>
-  <si>
-    <t>0-2259-7870, 0-2259-1865</t>
-  </si>
-  <si>
-    <t>89 หมู่ 3 ต.ในเมือง อ.เมืองร้อยเอ็ด จ.ร้อยเอ็ด 45150</t>
-  </si>
-  <si>
-    <t>02-259-7871-9</t>
-  </si>
-  <si>
     <t>A0270600106871</t>
   </si>
   <si>
@@ -253,6 +235,111 @@
   </si>
   <si>
     <t>1006.20.10005</t>
+  </si>
+  <si>
+    <t>SINGAPORE</t>
+  </si>
+  <si>
+    <t>0105532018537</t>
+  </si>
+  <si>
+    <t>บริษัท นำเข้าข้าว จำกัด</t>
+  </si>
+  <si>
+    <t>02-33301425-1</t>
+  </si>
+  <si>
+    <t>0-2335-5555</t>
+  </si>
+  <si>
+    <t>นายภานุ เยี่ยมมาก</t>
+  </si>
+  <si>
+    <t>02-252-1111-4</t>
+  </si>
+  <si>
+    <t>037498</t>
+  </si>
+  <si>
+    <t>พณ0308606000312</t>
+  </si>
+  <si>
+    <t>JAPAN</t>
+  </si>
+  <si>
+    <t>1355231415555</t>
+  </si>
+  <si>
+    <t>บริษัท เจแปน จำกัด</t>
+  </si>
+  <si>
+    <t>78 บางแค บางแค กรุงเทพมหานคร 10160</t>
+  </si>
+  <si>
+    <t>วัฒนา</t>
+  </si>
+  <si>
+    <t>0-2213-9851-2</t>
+  </si>
+  <si>
+    <t>0-2111-5453</t>
+  </si>
+  <si>
+    <t>นายมานี มีไห</t>
+  </si>
+  <si>
+    <t>31 ต.หล่มสัก อ.หล่มสัก เพชรบูรณ์ 41032</t>
+  </si>
+  <si>
+    <t>111 ต.เมือง อ.เมือง เลย 10333</t>
+  </si>
+  <si>
+    <t>02-332-1221-4</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>พณ0308606000313</t>
+  </si>
+  <si>
+    <t>037499</t>
+  </si>
+  <si>
+    <t>MALAYSIA</t>
+  </si>
+  <si>
+    <t>1211135829831</t>
+  </si>
+  <si>
+    <t>บริษัท พารวย จำกัด</t>
+  </si>
+  <si>
+    <t>พระราม9</t>
+  </si>
+  <si>
+    <t>0-2659-9243-1</t>
+  </si>
+  <si>
+    <t>0-2553-7788</t>
+  </si>
+  <si>
+    <t>นาย มาโนช กำจัดภัย</t>
+  </si>
+  <si>
+    <t>22 ต.บางแค อ.บางแค กรุงเทพมหานคร 10160</t>
+  </si>
+  <si>
+    <t>02-932-7441-9</t>
+  </si>
+  <si>
+    <t>MY</t>
+  </si>
+  <si>
+    <t>incoterm</t>
+  </si>
+  <si>
+    <t>CIF</t>
   </si>
 </sst>
 </file>
@@ -305,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -315,9 +402,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,18 +703,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD27"/>
+  <dimension ref="A1:AE27"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.75" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.75" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.75" style="1" bestFit="1" customWidth="1"/>
@@ -649,18 +733,19 @@
     <col min="20" max="20" width="10.625" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.125" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25.125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="15.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.125" style="1" customWidth="1"/>
-    <col min="31" max="16384" width="9" style="1"/>
+    <col min="23" max="23" width="12.5" style="1" customWidth="1"/>
+    <col min="24" max="24" width="15.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="25.125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="15.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.125" style="1" customWidth="1"/>
+    <col min="32" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
@@ -668,16 +753,16 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>27</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>9</v>
@@ -728,39 +813,42 @@
         <v>16</v>
       </c>
       <c r="W1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="X1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="3">
-        <v>42774</v>
-      </c>
-      <c r="D2" s="6">
+      <c r="C2" s="6">
         <v>42394</v>
+      </c>
+      <c r="D2" s="3">
+        <v>42775</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
@@ -805,7 +893,7 @@
         <v>46</v>
       </c>
       <c r="S2" s="3">
-        <v>42756</v>
+        <v>42787</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>38</v>
@@ -816,29 +904,32 @@
       <c r="V2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W2" s="1">
+      <c r="W2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="X2" s="1">
         <v>36.0852</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="Z2" s="1">
         <v>25000</v>
       </c>
-      <c r="Z2" s="1">
+      <c r="AA2" s="1">
         <v>1000</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AC2" s="1">
         <v>1440</v>
       </c>
-      <c r="AC2" s="1">
+      <c r="AD2" s="1">
         <v>1299067.2</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -846,10 +937,10 @@
         <v>53</v>
       </c>
       <c r="C3" s="6">
-        <v>42775</v>
+        <v>42761</v>
       </c>
       <c r="D3" s="6">
-        <v>42761</v>
+        <v>42776</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
@@ -861,31 +952,31 @@
         <v>28</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>46</v>
@@ -894,7 +985,7 @@
         <v>46</v>
       </c>
       <c r="S3" s="6">
-        <v>42757</v>
+        <v>42788</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>38</v>
@@ -905,40 +996,43 @@
       <c r="V3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W3" s="1">
+      <c r="W3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="X3" s="1">
         <v>37.0852</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Y3" s="1">
+      <c r="Z3" s="1">
         <v>300</v>
       </c>
-      <c r="Z3" s="1">
+      <c r="AA3" s="1">
         <v>10</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AB3" s="1">
+      <c r="AC3" s="1">
         <v>1440</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AD3" s="1">
         <v>1335067.2</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C4" s="6">
-        <v>42776</v>
+        <v>42763</v>
       </c>
       <c r="D4" s="6">
-        <v>43128</v>
+        <v>42778</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
@@ -950,40 +1044,40 @@
         <v>28</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="P4" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="Q4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="R4" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="S4" s="6">
-        <v>42758</v>
+        <v>42789</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>38</v>
@@ -994,223 +1088,393 @@
       <c r="V4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="W4" s="1">
+      <c r="W4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="X4" s="1">
         <v>35</v>
       </c>
-      <c r="X4" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y4" s="1">
+      <c r="Y4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z4" s="1">
         <v>5555</v>
       </c>
-      <c r="Z4" s="1">
+      <c r="AA4" s="1">
         <v>2345</v>
       </c>
-      <c r="AA4" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB4" s="1">
+      <c r="AB4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC4" s="1">
         <v>2000</v>
       </c>
-      <c r="AC4" s="1">
+      <c r="AD4" s="1">
         <v>388850</v>
       </c>
-      <c r="AD4" s="8"/>
-    </row>
-    <row r="5" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="I5" s="2"/>
-      <c r="S5" s="6"/>
-      <c r="U5" s="4"/>
-      <c r="AA5"/>
-      <c r="AD5" s="8"/>
-    </row>
-    <row r="6" spans="1:30" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="I6" s="2"/>
-      <c r="S6" s="6"/>
-      <c r="U6" s="4"/>
-      <c r="AD6" s="8"/>
-    </row>
-    <row r="7" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE4" s="8"/>
+    </row>
+    <row r="5" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="6">
+        <v>42763</v>
+      </c>
+      <c r="D5" s="6">
+        <v>42778</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="S5" s="6">
+        <v>42789</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="X5" s="1">
+        <v>35</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>50</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>2000</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>365020</v>
+      </c>
+      <c r="AE5" s="8"/>
+    </row>
+    <row r="6" spans="1:31" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="6">
+        <v>42764</v>
+      </c>
+      <c r="D6" s="6">
+        <v>42779</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="S6" s="6">
+        <v>42790</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="X6" s="1">
+        <v>36.0852</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>25000</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>1440</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>1299067.2</v>
+      </c>
+      <c r="AE6" s="8"/>
+    </row>
+    <row r="7" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="I7" s="2"/>
       <c r="S7" s="6"/>
       <c r="U7" s="4"/>
-      <c r="AD7" s="8"/>
-    </row>
-    <row r="8" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE7" s="8"/>
+    </row>
+    <row r="8" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="I8" s="2"/>
       <c r="S8" s="6"/>
       <c r="U8" s="4"/>
-      <c r="AD8" s="8"/>
-    </row>
-    <row r="9" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE8" s="8"/>
+    </row>
+    <row r="9" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="I9" s="2"/>
       <c r="S9" s="6"/>
       <c r="U9" s="4"/>
-      <c r="AD9" s="8"/>
-    </row>
-    <row r="10" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE9" s="8"/>
+    </row>
+    <row r="10" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="I10" s="2"/>
       <c r="S10" s="6"/>
       <c r="U10" s="4"/>
-      <c r="AD10" s="8"/>
-    </row>
-    <row r="11" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE10" s="8"/>
+    </row>
+    <row r="11" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="I11" s="2"/>
       <c r="S11" s="6"/>
       <c r="U11" s="4"/>
-      <c r="AD11" s="8"/>
-    </row>
-    <row r="12" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE11" s="8"/>
+    </row>
+    <row r="12" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="I12" s="2"/>
       <c r="S12" s="6"/>
       <c r="U12" s="4"/>
-      <c r="AD12" s="8"/>
-    </row>
-    <row r="13" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE12" s="8"/>
+    </row>
+    <row r="13" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="I13" s="2"/>
       <c r="S13" s="6"/>
       <c r="U13" s="4"/>
-      <c r="AD13" s="8"/>
-    </row>
-    <row r="14" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE13" s="8"/>
+    </row>
+    <row r="14" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="I14" s="2"/>
       <c r="S14" s="6"/>
       <c r="U14" s="4"/>
-      <c r="AD14" s="8"/>
-    </row>
-    <row r="15" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE14" s="8"/>
+    </row>
+    <row r="15" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="I15" s="2"/>
       <c r="S15" s="6"/>
       <c r="U15" s="4"/>
-      <c r="AD15" s="8"/>
-    </row>
-    <row r="16" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE15" s="8"/>
+    </row>
+    <row r="16" spans="1:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="I16" s="2"/>
       <c r="S16" s="6"/>
       <c r="U16" s="4"/>
-      <c r="AD16" s="8"/>
-    </row>
-    <row r="17" spans="2:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE16" s="8"/>
+    </row>
+    <row r="17" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="I17" s="2"/>
       <c r="S17" s="6"/>
       <c r="U17" s="4"/>
-      <c r="AD17" s="8"/>
-    </row>
-    <row r="18" spans="2:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE17" s="8"/>
+    </row>
+    <row r="18" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="I18" s="2"/>
       <c r="S18" s="6"/>
       <c r="U18" s="4"/>
-      <c r="AD18" s="8"/>
-    </row>
-    <row r="19" spans="2:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE18" s="8"/>
+    </row>
+    <row r="19" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="I19" s="2"/>
       <c r="S19" s="6"/>
       <c r="U19" s="4"/>
-      <c r="AD19" s="8"/>
-    </row>
-    <row r="20" spans="2:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE19" s="8"/>
+    </row>
+    <row r="20" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="I20" s="2"/>
       <c r="S20" s="6"/>
       <c r="U20" s="4"/>
-      <c r="AD20" s="8"/>
-    </row>
-    <row r="21" spans="2:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE20" s="8"/>
+    </row>
+    <row r="21" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="I21" s="2"/>
       <c r="S21" s="6"/>
       <c r="U21" s="4"/>
-      <c r="AD21" s="8"/>
-    </row>
-    <row r="22" spans="2:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE21" s="8"/>
+    </row>
+    <row r="22" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="I22" s="2"/>
       <c r="S22" s="6"/>
       <c r="U22" s="4"/>
-      <c r="AD22" s="8"/>
-    </row>
-    <row r="23" spans="2:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE22" s="8"/>
+    </row>
+    <row r="23" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="I23" s="2"/>
       <c r="S23" s="6"/>
       <c r="U23" s="4"/>
-      <c r="AD23" s="8"/>
-    </row>
-    <row r="24" spans="2:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE23" s="8"/>
+    </row>
+    <row r="24" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="I24" s="2"/>
       <c r="S24" s="6"/>
       <c r="U24" s="4"/>
-      <c r="AD24" s="8"/>
-    </row>
-    <row r="25" spans="2:30" ht="15" x14ac:dyDescent="0.25">
+      <c r="AE24" s="8"/>
+    </row>
+    <row r="25" spans="2:31" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="I25" s="2"/>
       <c r="S25" s="6"/>
       <c r="U25" s="4"/>
-      <c r="AD25" s="8"/>
-    </row>
-    <row r="26" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AE25" s="8"/>
+    </row>
+    <row r="26" spans="2:31" x14ac:dyDescent="0.2">
       <c r="S26" s="6"/>
     </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:31" x14ac:dyDescent="0.2">
       <c r="S27" s="6"/>
     </row>
   </sheetData>
@@ -1224,7 +1488,7 @@
   <dimension ref="A1:AD15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1292,7 +1556,7 @@
         <v>20</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
@@ -1312,7 +1576,7 @@
         <v>46</v>
       </c>
       <c r="F2" s="6">
-        <v>42756</v>
+        <v>42787</v>
       </c>
       <c r="G2" t="s">
         <v>42</v>
@@ -1339,30 +1603,30 @@
         <v>1000</v>
       </c>
       <c r="O2" s="6">
-        <v>42756</v>
+        <v>42787</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F3" s="6">
-        <v>42758</v>
+        <v>42789</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H3" t="s">
         <v>28</v>
@@ -1386,19 +1650,55 @@
         <v>2345</v>
       </c>
       <c r="O3" s="6">
-        <v>42756</v>
+        <v>42789</v>
       </c>
     </row>
     <row r="4" spans="1:30" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="C4" s="2"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4" s="6"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="N4"/>
-      <c r="O4" s="9"/>
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="6">
+        <v>42790</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="1">
+        <v>36.0852</v>
+      </c>
+      <c r="K4">
+        <v>36000</v>
+      </c>
+      <c r="L4">
+        <v>1299067.2</v>
+      </c>
+      <c r="M4">
+        <v>25000</v>
+      </c>
+      <c r="N4">
+        <v>1000</v>
+      </c>
+      <c r="O4" s="6">
+        <v>42790</v>
+      </c>
       <c r="S4" s="6"/>
       <c r="U4" s="4"/>
       <c r="AA4"/>

</xml_diff>